<commit_message>
Added Changes and files
</commit_message>
<xml_diff>
--- a/Dematic_MHE.xlsx
+++ b/Dematic_MHE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashokhulmanderi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashokhulmanderi/Desktop/PythonMhe/Python-Mhe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E215FD-CDBA-6640-ABD2-D03C47FCF0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC30CED-C7E3-3E47-BCCB-0BC24147CF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="9" xr2:uid="{54F012B5-AB48-4448-9ABE-36E1FBB0EEF6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="5" xr2:uid="{54F012B5-AB48-4448-9ABE-36E1FBB0EEF6}"/>
   </bookViews>
   <sheets>
     <sheet name="ORDERHDR" sheetId="18" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="254">
   <si>
     <t>Destination</t>
   </si>
@@ -702,9 +702,6 @@
     <t>Alphanumeric identifier that uniquely identifies the Container.  Corresponds to MAWM CrossReferenceLpnId for the outbound and to WM Pallet ID for inbound.</t>
   </si>
   <si>
-    <t>Container State</t>
-  </si>
-  <si>
     <t>DIVERTED or SCANNED or OPENED</t>
   </si>
   <si>
@@ -723,9 +720,6 @@
     <t>The load’s physical destination - Internal divert number</t>
   </si>
   <si>
-    <t>Customer Fields</t>
-  </si>
-  <si>
     <t>YYYYMMDD HHMMSS</t>
   </si>
   <si>
@@ -823,13 +817,40 @@
   </si>
   <si>
     <t>Log reason</t>
+  </si>
+  <si>
+    <t>&lt;STX&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ETX&gt;</t>
+  </si>
+  <si>
+    <t>MessageType</t>
+  </si>
+  <si>
+    <t>WaveID</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>ContainerID</t>
+  </si>
+  <si>
+    <t>ContainerState</t>
+  </si>
+  <si>
+    <t>LogicalDestination</t>
+  </si>
+  <si>
+    <t>PhysicalDestination</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -858,18 +879,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,37 +900,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA0A0A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA0A0A0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1014,15 +1008,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1130,115 +1115,82 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1580,7 +1532,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1632,7 +1584,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>142</v>
+        <v>245</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>10</v>
@@ -2502,7 +2454,7 @@
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="8" t="s">
-        <v>169</v>
+        <v>246</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>10</v>
@@ -2522,7 +2474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA1A7AB-D789-4521-A56D-B8EDC6C79BB4}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -3308,7 +3260,7 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
@@ -5152,10 +5104,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD59"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5371,7 +5323,7 @@
     </row>
     <row r="11" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
@@ -5447,7 +5399,7 @@
     </row>
     <row r="15" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
@@ -5487,7 +5439,7 @@
     </row>
     <row r="17" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>17</v>
+        <v>248</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>8</v>
@@ -5527,7 +5479,7 @@
     </row>
     <row r="19" spans="1:6" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>249</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>8</v>
@@ -5567,7 +5519,7 @@
     </row>
     <row r="21" spans="1:6" ht="71" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>62</v>
+        <v>250</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>8</v>
@@ -5607,7 +5559,7 @@
     </row>
     <row r="23" spans="1:6" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>8</v>
@@ -5616,13 +5568,13 @@
         <v>20</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
@@ -5797,7 +5749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>77</v>
       </c>
@@ -5814,10 +5766,10 @@
         <v>10</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>12</v>
       </c>
@@ -5837,9 +5789,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="43" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>127</v>
+        <v>252</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>8</v>
@@ -5848,16 +5800,16 @@
         <v>32</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>12</v>
       </c>
@@ -5877,9 +5829,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>130</v>
+        <v>253</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>8</v>
@@ -5888,383 +5840,120 @@
         <v>32</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F37" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="7">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="4">
+        <v>20</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="7">
-        <v>1</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="E39" s="4"/>
+      <c r="F39" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="4">
-        <v>20</v>
-      </c>
-      <c r="D40" s="5" t="s">
+    </row>
+    <row r="40" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="7">
-        <v>1</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="F41" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="8" t="s">
+      <c r="B42" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="8" t="s">
+      <c r="E42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:7" ht="43" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="42.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="E51" s="15"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="E52" s="15"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="E53" s="15"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="13"/>
-    </row>
-    <row r="55" spans="1:7" ht="54.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="E56" s="15"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="E57" s="15"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="50.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="27.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F6A986-AAD7-9C4E-8D40-BB0FF304AAAD}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6273,256 +5962,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="23" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="13" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="4" spans="1:7" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="24" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34" t="s">
-        <v>243</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="24" t="s">
-        <v>246</v>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="13" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:F15"/>
+  <mergeCells count="28">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>